<commit_message>
54 has been done
</commit_message>
<xml_diff>
--- a/ExtractedData.xlsx
+++ b/ExtractedData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\File\论文\Time-Synchronization-Paper-Repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\论文库\Time-Synchronization-Paper-Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CC9928-E417-46D1-A9D4-DA9AE1B22736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C48F2A5-5550-45B6-9542-BBE83044BB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Automotive" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="154">
   <si>
     <t>ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -589,33 +589,52 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>TA+PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Improved Clock Synchronization Start-Up Time for Ethernet AVB-Based In-Vehicle Networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diarra, A. and Hogenmueller, T. and Zimmermann, A. and Grzemba, A. and Khan, U. A. and Ieee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Proceedings of 2015 Ieee 20th Conference on Emerging Technologies &amp; Factory Automation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">formal mathematical analysis </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>formal mathematical analysis and simulation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>efficiency</t>
-  </si>
-  <si>
-    <t>TA+PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>formal mathematical analysis and proof of properties</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>the proposed method can resynchronize the network faster than the existing BMCA.</t>
-  </si>
-  <si>
-    <t>Improved Clock Synchronization Start-Up Time for Ethernet AVB-Based In-Vehicle Networks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Diarra, A. and Hogenmueller, T. and Zimmermann, A. and Grzemba, A. and Khan, U. A. and Ieee</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Proceedings of 2015 Ieee 20th Conference on Emerging Technologies &amp; Factory Automation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Clock Synchronization Start-Up Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>measurements on real implementations are planned to assess the real results.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">proposed several ways to reduce synchronization start-up time </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Modification of Sync frame size for neighbor rate ratio calculation      2.One-Step Messaging             3.Peer delay mechanism omission </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1011,11 +1030,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1454,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" s="3" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>50</v>
       </c>
@@ -1485,7 +1504,7 @@
       <c r="J7" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="6" t="s">
         <v>74</v>
       </c>
       <c r="M7" s="3" t="s">
@@ -1495,19 +1514,19 @@
         <v>141</v>
       </c>
       <c r="O7" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q7" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="P7" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>83</v>
+      <c r="R7" s="7" t="s">
+        <v>106</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="T7" s="3" t="s">
         <v>80</v>
@@ -1522,15 +1541,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" s="3" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>54</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>24</v>
@@ -1545,18 +1564,53 @@
         <v>27</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I8" s="3">
         <v>8</v>
       </c>
+      <c r="J8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="N8" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="P8" s="6"/>
+        <v>148</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="W8" s="3">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Y1" xr:uid="{A95080F3-5F0B-4AF5-B3D9-801697F94E6F}"/>

</xml_diff>